<commit_message>
Improve quiz management by adding features and database handling
Adds admin dashboard with database export/import, pagination, entry addition, and removes redundant access button.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/db_results.xlsx
+++ b/db_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +47,15 @@
     <t>2025-04-25 04:24:57</t>
   </si>
   <si>
+    <t>Deepa</t>
+  </si>
+  <si>
+    <t>I079692</t>
+  </si>
+  <si>
+    <t>2025-04-27 15:47:04</t>
+  </si>
+  <si>
     <t>Ajay</t>
   </si>
   <si>
@@ -54,6 +63,15 @@
   </si>
   <si>
     <t>2025-04-27 13:06:43</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>I999999</t>
+  </si>
+  <si>
+    <t>2025-04-27 15:43:16</t>
   </si>
 </sst>
 </file>
@@ -132,7 +150,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,7 +194,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>37.0</v>
+        <v>75.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>8</v>
@@ -202,7 +220,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>38.0</v>
+        <v>76.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>11</v>
@@ -220,10 +238,62 @@
         <v>5.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>26.0</v>
+        <v>21.0</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>77.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>78.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>80.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manage DB + sync fix
</commit_message>
<xml_diff>
--- a/db_results.xlsx
+++ b/db_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -23,7 +23,7 @@
     <t>I-Number</t>
   </si>
   <si>
-    <t>Score</t>
+    <t>Score (%)</t>
   </si>
   <si>
     <t>Total Questions</t>
@@ -32,10 +32,10 @@
     <t>Correct Answers</t>
   </si>
   <si>
-    <t>Duration (sec)</t>
-  </si>
-  <si>
-    <t>Completion Date</t>
+    <t>Time (sec)</t>
+  </si>
+  <si>
+    <t>Completed At</t>
   </si>
   <si>
     <t>TestExportImport</t>
@@ -72,6 +72,24 @@
   </si>
   <si>
     <t>2025-04-27 15:43:16</t>
+  </si>
+  <si>
+    <t>Meow</t>
+  </si>
+  <si>
+    <t>I07547</t>
+  </si>
+  <si>
+    <t>2025-04-27 21:41:00</t>
+  </si>
+  <si>
+    <t>Mona</t>
+  </si>
+  <si>
+    <t>I332232</t>
+  </si>
+  <si>
+    <t>2025-04-27 21:42:00</t>
   </si>
 </sst>
 </file>
@@ -111,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -119,50 +137,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="4.54296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.05078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.83984375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.0" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.15234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.4375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.19140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="15.9609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.95703125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="20.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -194,7 +194,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>75.0</v>
+        <v>105.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>8</v>
@@ -220,7 +220,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>76.0</v>
+        <v>106.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>11</v>
@@ -246,7 +246,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>77.0</v>
+        <v>107.0</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>14</v>
@@ -272,7 +272,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>78.0</v>
+        <v>108.0</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>17</v>
@@ -294,6 +294,58 @@
       </c>
       <c r="H5" t="s" s="0">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>109.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>110.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Db load from excel optimization
</commit_message>
<xml_diff>
--- a/db_results.xlsx
+++ b/db_results.xlsx
@@ -23,7 +23,7 @@
     <t>I-Number</t>
   </si>
   <si>
-    <t>Score (%)</t>
+    <t>Score</t>
   </si>
   <si>
     <t>Total Questions</t>
@@ -32,10 +32,10 @@
     <t>Correct Answers</t>
   </si>
   <si>
-    <t>Time (sec)</t>
-  </si>
-  <si>
-    <t>Completed At</t>
+    <t>Duration (sec)</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
   </si>
   <si>
     <t>TestExportImport</t>
@@ -129,13 +129,31 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -143,7 +161,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -159,10 +177,10 @@
     <col min="1" max="1" width="4.54296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.05078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.83984375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.15234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.0" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.4375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.19140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.95703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="15.9609375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="20.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Ui changes and gitignore
</commit_message>
<xml_diff>
--- a/db_results.xlsx
+++ b/db_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -65,15 +65,6 @@
     <t>2025-04-27 13:06:43</t>
   </si>
   <si>
-    <t>Test User</t>
-  </si>
-  <si>
-    <t>I999999</t>
-  </si>
-  <si>
-    <t>2025-04-27 15:43:16</t>
-  </si>
-  <si>
     <t>Meow</t>
   </si>
   <si>
@@ -90,6 +81,60 @@
   </si>
   <si>
     <t>2025-04-27 21:42:00</t>
+  </si>
+  <si>
+    <t>I0796921</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:12:00</t>
+  </si>
+  <si>
+    <t>312424</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:13:00</t>
+  </si>
+  <si>
+    <t>Meeryte</t>
+  </si>
+  <si>
+    <t>I012345566</t>
+  </si>
+  <si>
+    <t>Zumba</t>
+  </si>
+  <si>
+    <t>I5674572</t>
+  </si>
+  <si>
+    <t>ddfghd</t>
+  </si>
+  <si>
+    <t>2124235</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:14:00</t>
+  </si>
+  <si>
+    <t>24242352</t>
+  </si>
+  <si>
+    <t>2435325634</t>
+  </si>
+  <si>
+    <t>asdgs</t>
+  </si>
+  <si>
+    <t>343463</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:21:00</t>
+  </si>
+  <si>
+    <t>12415135</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:22:00</t>
   </si>
 </sst>
 </file>
@@ -168,7 +213,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,7 +221,7 @@
   <cols>
     <col min="1" max="1" width="4.54296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.05078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.83984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.70703125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.0" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.4375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.19140625" customWidth="true" bestFit="true"/>
@@ -290,7 +335,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>108.0</v>
+        <v>109.0</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>17</v>
@@ -299,16 +344,16 @@
         <v>18</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c r="E5" t="n" s="0">
         <v>5.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>60.0</v>
+        <v>12.0</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>19</v>
@@ -316,7 +361,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>109.0</v>
+        <v>110.0</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>20</v>
@@ -334,7 +379,7 @@
         <v>2.0</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>12.0</v>
+        <v>23.0</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>22</v>
@@ -342,28 +387,210 @@
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>110.0</v>
+        <v>112.0</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="D7" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D7" t="n" s="0">
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>113.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>114.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>115.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>116.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>117.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D12" t="n" s="0">
         <v>40.0</v>
       </c>
-      <c r="E7" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="F7" t="n" s="0">
+      <c r="E12" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F12" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="G7" t="n" s="0">
-        <v>23.0</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>25</v>
+      <c r="G12" t="n" s="0">
+        <v>224.0</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>118.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>119.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>